<commit_message>
add SEND_CMD byte and save status byte received in a static var to treat after in a function of sending
</commit_message>
<xml_diff>
--- a/Docs/Protocolo/Sensor Board V1.0 Protocol.xlsx
+++ b/Docs/Protocolo/Sensor Board V1.0 Protocol.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hardware 1\Desktop\Protocolo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hardware 1\Desktop\Meu_Sensor_Board\Sensor-Board\Docs\Protocolo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C1DEDC8-9C05-4604-A3E5-EEF92CCA21FA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95960255-64EF-47FE-93E3-E7EE32783AB2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="109">
   <si>
     <t>Byte 1</t>
   </si>
@@ -348,6 +348,12 @@
   </si>
   <si>
     <t>(0x0FF &amp; 0000XXXXb)</t>
+  </si>
+  <si>
+    <t>FLASH STORE</t>
+  </si>
+  <si>
+    <t>SEND FLAHS</t>
   </si>
 </sst>
 </file>
@@ -423,7 +429,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -802,6 +808,45 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -809,7 +854,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -908,6 +953,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1007,16 +1064,17 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1303,7 +1361,7 @@
   <dimension ref="B1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1318,25 +1376,25 @@
   <sheetData>
     <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="45" t="s">
+      <c r="C2" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="47"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="51"/>
     </row>
     <row r="3" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C4" s="42" t="s">
+      <c r="C4" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="44"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="48"/>
     </row>
     <row r="5" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="2" t="s">
@@ -1378,37 +1436,37 @@
         <v>9</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>10</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C8" s="42" t="s">
+      <c r="C8" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="43"/>
-      <c r="E8" s="43"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="43"/>
-      <c r="H8" s="44"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="47"/>
+      <c r="H8" s="48"/>
     </row>
     <row r="9" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="79" t="s">
         <v>0</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="80" t="s">
         <v>2</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="80" t="s">
         <v>3</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9" s="80" t="s">
         <v>4</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="H9" s="81" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1416,27 +1474,33 @@
       <c r="B10" s="40" t="s">
         <v>82</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="45" t="s">
         <v>15</v>
+      </c>
+      <c r="E10" s="82"/>
+      <c r="F10" s="82"/>
+      <c r="G10" s="82"/>
+      <c r="H10" s="83" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="11" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="E11" s="78" t="s">
+      <c r="E11" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="77" t="s">
+      <c r="F11" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="G11" s="75" t="s">
+      <c r="G11" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="H11" s="76" t="s">
+      <c r="H11" s="43" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1447,6 +1511,7 @@
     <mergeCell ref="C2:H2"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1469,21 +1534,21 @@
   <sheetData>
     <row r="1" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="48" t="s">
+      <c r="B2" s="52" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="50"/>
-      <c r="K2" s="51" t="s">
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="54"/>
+      <c r="K2" s="55" t="s">
         <v>46</v>
       </c>
-      <c r="L2" s="52"/>
-      <c r="M2" s="53"/>
+      <c r="L2" s="56"/>
+      <c r="M2" s="57"/>
     </row>
     <row r="3" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="10" t="s">
@@ -1583,21 +1648,21 @@
     </row>
     <row r="6" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="72" t="s">
+      <c r="B7" s="76" t="s">
         <v>57</v>
       </c>
-      <c r="C7" s="73"/>
-      <c r="D7" s="73"/>
-      <c r="E7" s="73"/>
-      <c r="F7" s="73"/>
-      <c r="G7" s="73"/>
-      <c r="H7" s="73"/>
-      <c r="I7" s="74"/>
-      <c r="K7" s="63" t="s">
+      <c r="C7" s="77"/>
+      <c r="D7" s="77"/>
+      <c r="E7" s="77"/>
+      <c r="F7" s="77"/>
+      <c r="G7" s="77"/>
+      <c r="H7" s="77"/>
+      <c r="I7" s="78"/>
+      <c r="K7" s="67" t="s">
         <v>77</v>
       </c>
-      <c r="L7" s="64"/>
-      <c r="M7" s="65"/>
+      <c r="L7" s="68"/>
+      <c r="M7" s="69"/>
     </row>
     <row r="8" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="31" t="s">
@@ -1805,21 +1870,21 @@
     </row>
     <row r="20" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="21" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="54" t="s">
+      <c r="B21" s="58" t="s">
         <v>45</v>
       </c>
-      <c r="C21" s="55"/>
-      <c r="D21" s="55"/>
-      <c r="E21" s="55"/>
-      <c r="F21" s="55"/>
-      <c r="G21" s="55"/>
-      <c r="H21" s="55"/>
-      <c r="I21" s="56"/>
-      <c r="K21" s="57" t="s">
+      <c r="C21" s="59"/>
+      <c r="D21" s="59"/>
+      <c r="E21" s="59"/>
+      <c r="F21" s="59"/>
+      <c r="G21" s="59"/>
+      <c r="H21" s="59"/>
+      <c r="I21" s="60"/>
+      <c r="K21" s="61" t="s">
         <v>78</v>
       </c>
-      <c r="L21" s="58"/>
-      <c r="M21" s="59"/>
+      <c r="L21" s="62"/>
+      <c r="M21" s="63"/>
     </row>
     <row r="22" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="19" t="s">
@@ -1983,21 +2048,21 @@
     </row>
     <row r="30" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="31" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="66" t="s">
+      <c r="B31" s="70" t="s">
         <v>54</v>
       </c>
-      <c r="C31" s="67"/>
-      <c r="D31" s="67"/>
-      <c r="E31" s="67"/>
-      <c r="F31" s="67"/>
-      <c r="G31" s="67"/>
-      <c r="H31" s="67"/>
-      <c r="I31" s="68"/>
-      <c r="K31" s="69" t="s">
+      <c r="C31" s="71"/>
+      <c r="D31" s="71"/>
+      <c r="E31" s="71"/>
+      <c r="F31" s="71"/>
+      <c r="G31" s="71"/>
+      <c r="H31" s="71"/>
+      <c r="I31" s="72"/>
+      <c r="K31" s="73" t="s">
         <v>79</v>
       </c>
-      <c r="L31" s="70"/>
-      <c r="M31" s="71"/>
+      <c r="L31" s="74"/>
+      <c r="M31" s="75"/>
     </row>
     <row r="32" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="16" t="s">
@@ -2161,16 +2226,16 @@
     </row>
     <row r="40" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="41" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B41" s="60" t="s">
+      <c r="B41" s="64" t="s">
         <v>71</v>
       </c>
-      <c r="C41" s="61"/>
-      <c r="D41" s="61"/>
-      <c r="E41" s="61"/>
-      <c r="F41" s="61"/>
-      <c r="G41" s="61"/>
-      <c r="H41" s="61"/>
-      <c r="I41" s="62"/>
+      <c r="C41" s="65"/>
+      <c r="D41" s="65"/>
+      <c r="E41" s="65"/>
+      <c r="F41" s="65"/>
+      <c r="G41" s="65"/>
+      <c r="H41" s="65"/>
+      <c r="I41" s="66"/>
     </row>
     <row r="42" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B42" s="34" t="s">

</xml_diff>

<commit_message>
change order of low-cal and cal in protocol
</commit_message>
<xml_diff>
--- a/Docs/Protocolo/Sensor Board V1.0 Protocol.xlsx
+++ b/Docs/Protocolo/Sensor Board V1.0 Protocol.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hardware 1\Desktop\Meu_Sensor_Board\Sensor-Board\Docs\Protocolo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25B1B4F5-DF3B-4014-AD31-89CB93A789A8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CECEDD2-B7B6-4537-8D86-D67BBE4F2E75}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -347,24 +347,6 @@
     <t>Byte 9</t>
   </si>
   <si>
-    <t>Cal MSB</t>
-  </si>
-  <si>
-    <t>Cal LSB</t>
-  </si>
-  <si>
-    <t>Low Cal MSB</t>
-  </si>
-  <si>
-    <t>High Cal MSB</t>
-  </si>
-  <si>
-    <t>Low Cal LSB</t>
-  </si>
-  <si>
-    <t>High Cal LSB</t>
-  </si>
-  <si>
     <t>Byte 10</t>
   </si>
   <si>
@@ -372,6 +354,24 @@
   </si>
   <si>
     <t>I2C Downstream (Master-to-Slave)</t>
+  </si>
+  <si>
+    <t>Low Cal (MSB)</t>
+  </si>
+  <si>
+    <t>Low Cal (LSB)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cal (MSB)</t>
+  </si>
+  <si>
+    <t>Cal (LSB)</t>
+  </si>
+  <si>
+    <t>High Cal (MSB)</t>
+  </si>
+  <si>
+    <t>High Cal (LSB)</t>
   </si>
 </sst>
 </file>
@@ -949,6 +949,32 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -958,6 +984,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1039,41 +1074,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -1358,7 +1358,7 @@
   <dimension ref="B2:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1367,74 +1367,76 @@
     <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="43" t="s">
-        <v>113</v>
-      </c>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
-      <c r="K3" s="44"/>
-      <c r="L3" s="45"/>
+      <c r="C3" s="53" t="s">
+        <v>107</v>
+      </c>
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
+      <c r="H3" s="54"/>
+      <c r="I3" s="54"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="54"/>
+      <c r="L3" s="55"/>
     </row>
     <row r="5" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C6" s="43" t="s">
-        <v>114</v>
-      </c>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="44"/>
-      <c r="G6" s="44"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="44"/>
-      <c r="J6" s="44"/>
-      <c r="K6" s="44"/>
-      <c r="L6" s="45"/>
+      <c r="C6" s="53" t="s">
+        <v>108</v>
+      </c>
+      <c r="D6" s="54"/>
+      <c r="E6" s="54"/>
+      <c r="F6" s="54"/>
+      <c r="G6" s="54"/>
+      <c r="H6" s="54"/>
+      <c r="I6" s="54"/>
+      <c r="J6" s="54"/>
+      <c r="K6" s="54"/>
+      <c r="L6" s="55"/>
     </row>
     <row r="7" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="79" t="s">
+      <c r="C7" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="75" t="s">
+      <c r="D7" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="75" t="s">
+      <c r="E7" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="75" t="s">
+      <c r="F7" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="G7" s="75" t="s">
+      <c r="G7" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="H7" s="80" t="s">
+      <c r="H7" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="I7" s="77" t="s">
+      <c r="I7" s="47" t="s">
         <v>103</v>
       </c>
-      <c r="J7" s="77" t="s">
+      <c r="J7" s="47" t="s">
         <v>104</v>
       </c>
-      <c r="K7" s="77" t="s">
+      <c r="K7" s="47" t="s">
         <v>105</v>
       </c>
-      <c r="L7" s="78" t="s">
-        <v>112</v>
+      <c r="L7" s="48" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1451,74 +1453,74 @@
         <v>7</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="J8" s="73" t="s">
-        <v>109</v>
-      </c>
-      <c r="K8" s="73" t="s">
-        <v>111</v>
-      </c>
-      <c r="L8" s="74" t="s">
+        <v>112</v>
+      </c>
+      <c r="J8" s="43" t="s">
+        <v>113</v>
+      </c>
+      <c r="K8" s="43" t="s">
+        <v>114</v>
+      </c>
+      <c r="L8" s="44" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="9" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="40"/>
-      <c r="C10" s="43" t="s">
+      <c r="C10" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="44"/>
-      <c r="E10" s="44"/>
-      <c r="F10" s="44"/>
-      <c r="G10" s="44"/>
-      <c r="H10" s="44"/>
-      <c r="I10" s="44"/>
-      <c r="J10" s="44"/>
-      <c r="K10" s="44"/>
-      <c r="L10" s="45"/>
+      <c r="D10" s="54"/>
+      <c r="E10" s="54"/>
+      <c r="F10" s="54"/>
+      <c r="G10" s="54"/>
+      <c r="H10" s="54"/>
+      <c r="I10" s="54"/>
+      <c r="J10" s="54"/>
+      <c r="K10" s="54"/>
+      <c r="L10" s="55"/>
     </row>
     <row r="11" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="81"/>
+      <c r="B11" s="51"/>
       <c r="C11" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D11" s="76" t="s">
+      <c r="D11" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="E11" s="75" t="s">
+      <c r="E11" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="F11" s="75" t="s">
+      <c r="F11" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="G11" s="75" t="s">
+      <c r="G11" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="H11" s="75" t="s">
+      <c r="H11" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="I11" s="77" t="s">
+      <c r="I11" s="47" t="s">
         <v>103</v>
       </c>
-      <c r="J11" s="77" t="s">
+      <c r="J11" s="47" t="s">
         <v>104</v>
       </c>
-      <c r="K11" s="77" t="s">
+      <c r="K11" s="47" t="s">
         <v>105</v>
       </c>
-      <c r="L11" s="78" t="s">
-        <v>112</v>
+      <c r="L11" s="48" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1528,21 +1530,21 @@
       <c r="C12" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="82"/>
-      <c r="E12" s="83"/>
-      <c r="F12" s="83"/>
-      <c r="G12" s="83"/>
-      <c r="H12" s="83"/>
-      <c r="I12" s="83"/>
-      <c r="J12" s="83"/>
-      <c r="K12" s="83"/>
-      <c r="L12" s="84"/>
+      <c r="D12" s="56"/>
+      <c r="E12" s="57"/>
+      <c r="F12" s="57"/>
+      <c r="G12" s="57"/>
+      <c r="H12" s="57"/>
+      <c r="I12" s="57"/>
+      <c r="J12" s="57"/>
+      <c r="K12" s="57"/>
+      <c r="L12" s="58"/>
     </row>
     <row r="13" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="41" t="s">
         <v>78</v>
       </c>
-      <c r="C13" s="85"/>
+      <c r="C13" s="52"/>
       <c r="D13" s="3" t="s">
         <v>11</v>
       </c>
@@ -1550,24 +1552,24 @@
         <v>10</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="J13" s="73" t="s">
-        <v>109</v>
-      </c>
-      <c r="K13" s="73" t="s">
-        <v>111</v>
-      </c>
-      <c r="L13" s="74" t="s">
+        <v>112</v>
+      </c>
+      <c r="J13" s="43" t="s">
+        <v>113</v>
+      </c>
+      <c r="K13" s="43" t="s">
+        <v>114</v>
+      </c>
+      <c r="L13" s="44" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1605,21 +1607,21 @@
   <sheetData>
     <row r="1" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="59" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="48"/>
-      <c r="K2" s="49" t="s">
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="61"/>
+      <c r="K2" s="62" t="s">
         <v>41</v>
       </c>
-      <c r="L2" s="50"/>
-      <c r="M2" s="51"/>
+      <c r="L2" s="63"/>
+      <c r="M2" s="64"/>
     </row>
     <row r="3" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="8" t="s">
@@ -1719,21 +1721,21 @@
     </row>
     <row r="6" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="70" t="s">
+      <c r="B7" s="83" t="s">
         <v>52</v>
       </c>
-      <c r="C7" s="71"/>
-      <c r="D7" s="71"/>
-      <c r="E7" s="71"/>
-      <c r="F7" s="71"/>
-      <c r="G7" s="71"/>
-      <c r="H7" s="71"/>
-      <c r="I7" s="72"/>
-      <c r="K7" s="61" t="s">
+      <c r="C7" s="84"/>
+      <c r="D7" s="84"/>
+      <c r="E7" s="84"/>
+      <c r="F7" s="84"/>
+      <c r="G7" s="84"/>
+      <c r="H7" s="84"/>
+      <c r="I7" s="85"/>
+      <c r="K7" s="74" t="s">
         <v>72</v>
       </c>
-      <c r="L7" s="62"/>
-      <c r="M7" s="63"/>
+      <c r="L7" s="75"/>
+      <c r="M7" s="76"/>
     </row>
     <row r="8" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="29" t="s">
@@ -1941,21 +1943,21 @@
     </row>
     <row r="20" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="21" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="52" t="s">
+      <c r="B21" s="65" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="53"/>
-      <c r="D21" s="53"/>
-      <c r="E21" s="53"/>
-      <c r="F21" s="53"/>
-      <c r="G21" s="53"/>
-      <c r="H21" s="53"/>
-      <c r="I21" s="54"/>
-      <c r="K21" s="55" t="s">
+      <c r="C21" s="66"/>
+      <c r="D21" s="66"/>
+      <c r="E21" s="66"/>
+      <c r="F21" s="66"/>
+      <c r="G21" s="66"/>
+      <c r="H21" s="66"/>
+      <c r="I21" s="67"/>
+      <c r="K21" s="68" t="s">
         <v>73</v>
       </c>
-      <c r="L21" s="56"/>
-      <c r="M21" s="57"/>
+      <c r="L21" s="69"/>
+      <c r="M21" s="70"/>
     </row>
     <row r="22" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="17" t="s">
@@ -2119,21 +2121,21 @@
     </row>
     <row r="30" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="31" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="64" t="s">
+      <c r="B31" s="77" t="s">
         <v>49</v>
       </c>
-      <c r="C31" s="65"/>
-      <c r="D31" s="65"/>
-      <c r="E31" s="65"/>
-      <c r="F31" s="65"/>
-      <c r="G31" s="65"/>
-      <c r="H31" s="65"/>
-      <c r="I31" s="66"/>
-      <c r="K31" s="67" t="s">
+      <c r="C31" s="78"/>
+      <c r="D31" s="78"/>
+      <c r="E31" s="78"/>
+      <c r="F31" s="78"/>
+      <c r="G31" s="78"/>
+      <c r="H31" s="78"/>
+      <c r="I31" s="79"/>
+      <c r="K31" s="80" t="s">
         <v>74</v>
       </c>
-      <c r="L31" s="68"/>
-      <c r="M31" s="69"/>
+      <c r="L31" s="81"/>
+      <c r="M31" s="82"/>
     </row>
     <row r="32" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="14" t="s">
@@ -2297,16 +2299,16 @@
     </row>
     <row r="40" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="41" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B41" s="58" t="s">
+      <c r="B41" s="71" t="s">
         <v>66</v>
       </c>
-      <c r="C41" s="59"/>
-      <c r="D41" s="59"/>
-      <c r="E41" s="59"/>
-      <c r="F41" s="59"/>
-      <c r="G41" s="59"/>
-      <c r="H41" s="59"/>
-      <c r="I41" s="60"/>
+      <c r="C41" s="72"/>
+      <c r="D41" s="72"/>
+      <c r="E41" s="72"/>
+      <c r="F41" s="72"/>
+      <c r="G41" s="72"/>
+      <c r="H41" s="72"/>
+      <c r="I41" s="73"/>
     </row>
     <row r="42" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B42" s="32" t="s">

</xml_diff>